<commit_message>
Seção 3 (Experimentos e Resultados)
</commit_message>
<xml_diff>
--- a/resultados/result.xlsx
+++ b/resultados/result.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="20">
   <si>
     <t>D</t>
   </si>
@@ -74,10 +74,7 @@
     <t>Resources Recall (Ration of retrieved resources by retrieved sf)</t>
   </si>
   <si>
-    <t>Verifications</t>
-  </si>
-  <si>
-    <t>Linha21 – Linha22 (Deve ser maior ou igual a zero)</t>
+    <t>Número de anotações L26 + L27</t>
   </si>
 </sst>
 </file>
@@ -87,7 +84,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -131,13 +128,6 @@
       <charset val="1"/>
       <family val="2"/>
       <color rgb="00222222"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00FF0000"/>
       <sz val="12"/>
     </font>
   </fonts>
@@ -278,7 +268,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="4" numFmtId="164" xfId="0">
@@ -325,7 +315,6 @@
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -406,7 +395,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A13" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <selection activeCell="A16" activeCellId="0" pane="topLeft" sqref="A16"/>
+      <selection activeCell="A33" activeCellId="0" pane="topLeft" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -1381,9 +1370,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="32">
-      <c r="A32" s="24" t="s">
-        <v>19</v>
-      </c>
+      <c r="A32" s="24"/>
       <c r="B32" s="25"/>
       <c r="C32" s="25"/>
       <c r="D32" s="25"/>
@@ -1399,55 +1386,55 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B33" s="0" t="n">
-        <f aca="false">B25-B26</f>
-        <v>93</v>
+        <f aca="false">B26+B27</f>
+        <v>185</v>
       </c>
       <c r="C33" s="0" t="n">
-        <f aca="false">C25-C26</f>
-        <v>60</v>
+        <f aca="false">C26+C27</f>
+        <v>84</v>
       </c>
       <c r="D33" s="0" t="n">
-        <f aca="false">D25-D26</f>
-        <v>78</v>
+        <f aca="false">D26+D27</f>
+        <v>267</v>
       </c>
       <c r="E33" s="0" t="n">
-        <f aca="false">E25-E26</f>
-        <v>4</v>
+        <f aca="false">E26+E27</f>
+        <v>255</v>
       </c>
       <c r="F33" s="0" t="n">
-        <f aca="false">F25-F26</f>
-        <v>717</v>
+        <f aca="false">F26+F27</f>
+        <v>15270</v>
       </c>
       <c r="G33" s="0" t="n">
-        <f aca="false">G25-G26</f>
-        <v>468</v>
-      </c>
-      <c r="H33" s="26" t="n">
-        <f aca="false">H25-H26</f>
-        <v>-453</v>
-      </c>
-      <c r="I33" s="26" t="n">
-        <f aca="false">I25-I26</f>
-        <v>-5601</v>
+        <f aca="false">G26+G27</f>
+        <v>4977</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <f aca="false">H26+H27</f>
+        <v>19189</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <f aca="false">I26+I27</f>
+        <v>19344</v>
       </c>
       <c r="J33" s="0" t="n">
-        <f aca="false">J25-J26</f>
-        <v>334</v>
+        <f aca="false">J26+J27</f>
+        <v>1642</v>
       </c>
       <c r="K33" s="0" t="n">
-        <f aca="false">K25-K26</f>
-        <v>187</v>
+        <f aca="false">K26+K27</f>
+        <v>618</v>
       </c>
       <c r="L33" s="0" t="n">
-        <f aca="false">L25-L26</f>
-        <v>81</v>
-      </c>
-      <c r="M33" s="26" t="n">
-        <f aca="false">M25-M26</f>
-        <v>-567</v>
+        <f aca="false">L26+L27</f>
+        <v>2387</v>
+      </c>
+      <c r="M33" s="0" t="n">
+        <f aca="false">M26+M27</f>
+        <v>2386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>